<commit_message>
completed reserve book issue book and return book functionality
</commit_message>
<xml_diff>
--- a/lms_books.xlsx
+++ b/lms_books.xlsx
@@ -470,7 +470,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
@@ -518,7 +518,7 @@
       </c>
       <c r="H1" s="4" t="inlineStr">
         <is>
-          <t>User_1</t>
+          <t>Issued By</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>George Owell</t>
+          <t>George Orwell</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
@@ -541,14 +541,14 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>Issued</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="F2" s="7" t="n">
-        <v>44908</v>
+        <v>0</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>44910</v>
+        <v>0</v>
       </c>
       <c r="H2" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
added some librarian functionality and some functoinality to shelf
</commit_message>
<xml_diff>
--- a/lms_books.xlsx
+++ b/lms_books.xlsx
@@ -541,17 +541,19 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Reserved</t>
         </is>
       </c>
       <c r="F2" s="7" t="n">
-        <v>0</v>
+        <v>44910</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" s="4" t="n">
-        <v>0</v>
+        <v>45272</v>
+      </c>
+      <c r="H2" s="4" t="inlineStr">
+        <is>
+          <t>User_1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added remove book and add book functoinality
</commit_message>
<xml_diff>
--- a/lms_books.xlsx
+++ b/lms_books.xlsx
@@ -16,8 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -75,7 +76,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -96,6 +97,9 @@
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -523,10 +527,12 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="5">
-      <c r="A2" s="4" t="n">
-        <v>1984</v>
-      </c>
-      <c r="B2" s="6" t="n">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>1984</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
         <v>9780451524935</v>
       </c>
       <c r="C2" s="4" t="inlineStr">
@@ -541,19 +547,17 @@
       </c>
       <c r="E2" s="4" t="inlineStr">
         <is>
-          <t>Reserved</t>
-        </is>
-      </c>
-      <c r="F2" s="7" t="n">
-        <v>44910</v>
-      </c>
-      <c r="G2" s="7" t="n">
-        <v>45272</v>
-      </c>
-      <c r="H2" s="4" t="inlineStr">
-        <is>
-          <t>User_1</t>
-        </is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>